<commit_message>
primeiro commit branch nova
alteracoes cores e letra
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FEA468-86A8-475A-B363-645AD1566726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132538A3-16FA-4DD8-BD22-2C9292515279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,14 +30,14 @@
     <t>TESTE</t>
   </si>
   <si>
-    <t>a</t>
+    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,6 +48,7 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -55,6 +56,15 @@
     <font>
       <b/>
       <sz val="30"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +79,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,16 +154,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -439,116 +450,116 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>